<commit_message>
wip:ya se guardan datos en carpewtas y en base de datos
</commit_message>
<xml_diff>
--- a/imagenes_guardadas/archivo_modificado_RESGUARDO.xlsx
+++ b/imagenes_guardadas/archivo_modificado_RESGUARDO.xlsx
@@ -10,14 +10,14 @@
     <sheet name="plantilla" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'plantilla'!$B$1:$M$81</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'plantilla'!$B$1:$M$76</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>Automóviles y Camiones Rivera, S.A. de C.V.</t>
   </si>
@@ -28,13 +28,13 @@
     <t>No. de Resguardo:</t>
   </si>
   <si>
-    <t>02-00 PC-COMPLETA</t>
+    <t>011-00 OTRO</t>
   </si>
   <si>
     <t>Fecha de resguardo:</t>
   </si>
   <si>
-    <t>06-FEBRERO-2025</t>
+    <t>07-FEBRERO-2025</t>
   </si>
   <si>
     <t>De acuerdo con la “AS-DV-002. Uso de recursos informáticos”, me comprometo a utilizar el hardware y/o software que se me asigno, exclusivamente para actividades relacionadas con los negocios de la empresa, así como a cuidarlo y mantenerlo en buen estado</t>
@@ -46,12 +46,12 @@
     <t>Equipo ACR</t>
   </si>
   <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>Equipo Externo</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>CANT</t>
   </si>
   <si>
@@ -70,16 +70,19 @@
     <t>Inv. Físico</t>
   </si>
   <si>
-    <t>ASDAS</t>
-  </si>
-  <si>
-    <t>ASD</t>
+    <t>ASDFSA</t>
+  </si>
+  <si>
+    <t>ASDAF</t>
+  </si>
+  <si>
+    <t>ADSF</t>
+  </si>
+  <si>
+    <t>ADFAS</t>
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>PERRO</t>
   </si>
   <si>
     <t>CARACTERISTICAS DEL SOFTWARE</t>
@@ -114,7 +117,7 @@
     <t>Julio Castillo Valerdi</t>
   </si>
   <si>
-    <t>Soporte 2</t>
+    <t>Hj</t>
   </si>
   <si>
     <t>Soporte1</t>
@@ -567,6 +570,9 @@
     <xf xfId="0" fontId="1" numFmtId="49" fillId="3" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="1" numFmtId="49" fillId="3" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -685,9 +691,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="8" numFmtId="0" fillId="2" borderId="20" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="49" fillId="3" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -742,13 +745,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1102,10 +1105,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N81"/>
+  <dimension ref="A1:N76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="85" view="pageBreakPreview" showGridLines="true" showRowColHeaders="1" topLeftCell="B2">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="85" view="pageBreakPreview" showGridLines="true" showRowColHeaders="1" topLeftCell="B65">
+      <selection activeCell="A70" sqref="A70:XFD71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1159,19 +1162,19 @@
       <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="66" t="s">
+      <c r="L7" s="26" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:14" customHeight="1" ht="7.5"/>
     <row r="9" spans="1:14" customHeight="1" ht="6">
       <c r="A9" s="2"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
       <c r="K9" s="7"/>
       <c r="L9" s="21"/>
       <c r="M9" s="3"/>
@@ -1193,110 +1196,110 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2"/>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
     </row>
     <row r="12" spans="1:14" customHeight="1" ht="7.5">
       <c r="A12" s="2"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
     </row>
     <row r="13" spans="1:14" customHeight="1" ht="7.5">
       <c r="A13" s="2"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
     </row>
     <row r="14" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
     </row>
     <row r="16" spans="1:14" customHeight="1" ht="0.75"/>
     <row r="17" spans="1:14" customHeight="1" ht="18.75">
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
     </row>
     <row r="18" spans="1:14" customHeight="1" ht="7.5"/>
     <row r="19" spans="1:14" s="3" customFormat="1">
       <c r="B19" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="F19" s="32" t="s">
+      <c r="C19" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="13" t="s">
+      <c r="F19" s="33" t="s">
         <v>10</v>
       </c>
+      <c r="G19" s="33"/>
+      <c r="H19" s="13"/>
       <c r="L19" s="22"/>
     </row>
     <row r="20" spans="1:14" customHeight="1" ht="7.5"/>
@@ -1305,18 +1308,18 @@
       <c r="B21" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="29" t="s">
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="32"/>
       <c r="K21" s="12" t="s">
         <v>14</v>
       </c>
@@ -1332,119 +1335,83 @@
       <c r="B22" s="18">
         <v>1</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="37"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="38"/>
       <c r="K22" s="19" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L22" s="25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="M22" s="19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:14" customHeight="1" ht="26.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="18">
-        <v>1</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="L23" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="M23" s="19" t="s">
-        <v>19</v>
-      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="19"/>
     </row>
     <row r="24" spans="1:14" customHeight="1" ht="26.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="18">
-        <v>1</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="L24" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="M24" s="19" t="s">
-        <v>19</v>
-      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="19"/>
     </row>
     <row r="25" spans="1:14" customHeight="1" ht="26.25">
-      <c r="B25" s="18">
-        <v>1</v>
-      </c>
-      <c r="C25" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="M25" s="19" t="s">
-        <v>19</v>
-      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="19"/>
     </row>
     <row r="26" spans="1:14" customHeight="1" ht="26.25">
       <c r="A26" s="2"/>
       <c r="B26" s="18"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="37"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="38"/>
       <c r="K26" s="19"/>
       <c r="L26" s="24"/>
       <c r="M26" s="19"/>
@@ -1461,48 +1428,48 @@
     </row>
     <row r="28" spans="1:14" customHeight="1" ht="3">
       <c r="A28" s="2"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="2"/>
       <c r="E28" s="7"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="21"/>
     </row>
     <row r="29" spans="1:14" customHeight="1" ht="7.5" hidden="true">
-      <c r="B29" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
+      <c r="B29" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
     </row>
     <row r="30" spans="1:14" customHeight="1" ht="13.5">
       <c r="A30" s="2"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
     </row>
     <row r="31" spans="1:14" customHeight="1" ht="7.5">
       <c r="B31" s="3"/>
@@ -1517,86 +1484,86 @@
     </row>
     <row r="32" spans="1:14" customHeight="1" ht="14.45">
       <c r="A32" s="2"/>
-      <c r="B32" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
+      <c r="B32" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="34"/>
+      <c r="L32" s="34"/>
+      <c r="M32" s="34"/>
     </row>
     <row r="33" spans="1:14" customHeight="1" ht="14.45">
       <c r="A33" s="2"/>
       <c r="B33" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
       <c r="K33" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L33" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="M33" s="50"/>
+      <c r="L33" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="M33" s="51"/>
     </row>
     <row r="34" spans="1:14" customHeight="1" ht="14.45">
       <c r="A34" s="3"/>
       <c r="B34" s="16"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="54"/>
-      <c r="H34" s="54"/>
-      <c r="I34" s="54"/>
-      <c r="J34" s="55"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="55"/>
+      <c r="J34" s="56"/>
       <c r="K34" s="17"/>
-      <c r="L34" s="51"/>
-      <c r="M34" s="52"/>
+      <c r="L34" s="52"/>
+      <c r="M34" s="53"/>
     </row>
     <row r="35" spans="1:14" customHeight="1" ht="14.45">
       <c r="B35" s="16"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="54"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="54"/>
-      <c r="I35" s="54"/>
-      <c r="J35" s="55"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="55"/>
+      <c r="J35" s="56"/>
       <c r="K35" s="17"/>
-      <c r="L35" s="51"/>
-      <c r="M35" s="52"/>
+      <c r="L35" s="52"/>
+      <c r="M35" s="53"/>
     </row>
     <row r="36" spans="1:14" customHeight="1" ht="14.45">
       <c r="B36" s="16"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="56"/>
-      <c r="J36" s="52"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="57"/>
+      <c r="J36" s="53"/>
       <c r="K36" s="17"/>
-      <c r="L36" s="51"/>
-      <c r="M36" s="52"/>
+      <c r="L36" s="52"/>
+      <c r="M36" s="53"/>
     </row>
     <row r="37" spans="1:14" customHeight="1" ht="3.75"/>
     <row r="38" spans="1:14" customHeight="1" ht="13.5" hidden="true">
@@ -1610,376 +1577,376 @@
     </row>
     <row r="41" spans="1:14" customHeight="1" ht="6"/>
     <row r="42" spans="1:14" customHeight="1" ht="13.5">
-      <c r="B42" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="42"/>
-      <c r="J42" s="42"/>
-      <c r="K42" s="42"/>
-      <c r="L42" s="42"/>
-      <c r="M42" s="42"/>
+      <c r="B42" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="43"/>
+      <c r="M42" s="43"/>
     </row>
     <row r="43" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B43" s="42"/>
-      <c r="C43" s="42"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
-      <c r="K43" s="42"/>
-      <c r="L43" s="42"/>
-      <c r="M43" s="42"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
+      <c r="K43" s="43"/>
+      <c r="L43" s="43"/>
+      <c r="M43" s="43"/>
     </row>
     <row r="44" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B44" s="42"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="42"/>
-      <c r="K44" s="42"/>
-      <c r="L44" s="42"/>
-      <c r="M44" s="42"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="43"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
+      <c r="K44" s="43"/>
+      <c r="L44" s="43"/>
+      <c r="M44" s="43"/>
     </row>
     <row r="45" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B45" s="42"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42"/>
-      <c r="J45" s="42"/>
-      <c r="K45" s="42"/>
-      <c r="L45" s="42"/>
-      <c r="M45" s="42"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="43"/>
+      <c r="M45" s="43"/>
     </row>
     <row r="46" spans="1:14">
-      <c r="B46" s="42"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="42"/>
-      <c r="J46" s="42"/>
-      <c r="K46" s="42"/>
-      <c r="L46" s="42"/>
-      <c r="M46" s="42"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="43"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="43"/>
+      <c r="M46" s="43"/>
     </row>
     <row r="47" spans="1:14" customHeight="1" ht="12">
-      <c r="B47" s="42"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="42"/>
-      <c r="F47" s="42"/>
-      <c r="G47" s="42"/>
-      <c r="H47" s="42"/>
-      <c r="I47" s="42"/>
-      <c r="J47" s="42"/>
-      <c r="K47" s="42"/>
-      <c r="L47" s="42"/>
-      <c r="M47" s="42"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="43"/>
+      <c r="J47" s="43"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="43"/>
+      <c r="M47" s="43"/>
     </row>
     <row r="48" spans="1:14" customHeight="1" ht="13.5">
-      <c r="B48" s="42"/>
-      <c r="C48" s="42"/>
-      <c r="D48" s="42"/>
-      <c r="E48" s="42"/>
-      <c r="F48" s="42"/>
-      <c r="G48" s="42"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="42"/>
-      <c r="J48" s="42"/>
-      <c r="K48" s="42"/>
-      <c r="L48" s="42"/>
-      <c r="M48" s="42"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="43"/>
+      <c r="M48" s="43"/>
     </row>
     <row r="49" spans="1:14" customHeight="1" ht="3.75">
-      <c r="B49" s="42"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="42"/>
-      <c r="J49" s="42"/>
-      <c r="K49" s="42"/>
-      <c r="L49" s="42"/>
-      <c r="M49" s="42"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="43"/>
+      <c r="F49" s="43"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="43"/>
+      <c r="I49" s="43"/>
+      <c r="J49" s="43"/>
+      <c r="K49" s="43"/>
+      <c r="L49" s="43"/>
+      <c r="M49" s="43"/>
     </row>
     <row r="50" spans="1:14" customHeight="1" ht="13.5">
-      <c r="B50" s="42"/>
-      <c r="C50" s="42"/>
-      <c r="D50" s="42"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="42"/>
-      <c r="G50" s="42"/>
-      <c r="H50" s="42"/>
-      <c r="I50" s="42"/>
-      <c r="J50" s="42"/>
-      <c r="K50" s="42"/>
-      <c r="L50" s="42"/>
-      <c r="M50" s="42"/>
+      <c r="B50" s="43"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="43"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="43"/>
+      <c r="I50" s="43"/>
+      <c r="J50" s="43"/>
+      <c r="K50" s="43"/>
+      <c r="L50" s="43"/>
+      <c r="M50" s="43"/>
     </row>
     <row r="51" spans="1:14" customHeight="1" ht="3.75">
-      <c r="B51" s="42"/>
-      <c r="C51" s="42"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="42"/>
-      <c r="J51" s="42"/>
-      <c r="K51" s="42"/>
-      <c r="L51" s="42"/>
-      <c r="M51" s="42"/>
+      <c r="B51" s="43"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="43"/>
+      <c r="J51" s="43"/>
+      <c r="K51" s="43"/>
+      <c r="L51" s="43"/>
+      <c r="M51" s="43"/>
     </row>
     <row r="52" spans="1:14" customHeight="1" ht="24">
-      <c r="B52" s="42"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="42"/>
-      <c r="F52" s="42"/>
-      <c r="G52" s="42"/>
-      <c r="H52" s="42"/>
-      <c r="I52" s="42"/>
-      <c r="J52" s="42"/>
-      <c r="K52" s="42"/>
-      <c r="L52" s="42"/>
-      <c r="M52" s="42"/>
+      <c r="B52" s="43"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="43"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="43"/>
+      <c r="I52" s="43"/>
+      <c r="J52" s="43"/>
+      <c r="K52" s="43"/>
+      <c r="L52" s="43"/>
+      <c r="M52" s="43"/>
     </row>
     <row r="53" spans="1:14" customHeight="1" ht="3.75" hidden="true">
-      <c r="B53" s="42"/>
-      <c r="C53" s="42"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="42"/>
-      <c r="H53" s="42"/>
-      <c r="I53" s="42"/>
-      <c r="J53" s="42"/>
-      <c r="K53" s="42"/>
-      <c r="L53" s="42"/>
-      <c r="M53" s="42"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="43"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="43"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="43"/>
+      <c r="I53" s="43"/>
+      <c r="J53" s="43"/>
+      <c r="K53" s="43"/>
+      <c r="L53" s="43"/>
+      <c r="M53" s="43"/>
     </row>
     <row r="54" spans="1:14" customHeight="1" ht="13.5" hidden="true">
-      <c r="B54" s="42"/>
-      <c r="C54" s="42"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="42"/>
-      <c r="F54" s="42"/>
-      <c r="G54" s="42"/>
-      <c r="H54" s="42"/>
-      <c r="I54" s="42"/>
-      <c r="J54" s="42"/>
-      <c r="K54" s="42"/>
-      <c r="L54" s="42"/>
-      <c r="M54" s="42"/>
+      <c r="B54" s="43"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="43"/>
+      <c r="E54" s="43"/>
+      <c r="F54" s="43"/>
+      <c r="G54" s="43"/>
+      <c r="H54" s="43"/>
+      <c r="I54" s="43"/>
+      <c r="J54" s="43"/>
+      <c r="K54" s="43"/>
+      <c r="L54" s="43"/>
+      <c r="M54" s="43"/>
     </row>
     <row r="55" spans="1:14" customHeight="1" ht="3.75">
       <c r="F55" s="3"/>
     </row>
     <row r="56" spans="1:14" customHeight="1" ht="13.5">
-      <c r="B56" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="C56" s="44"/>
-      <c r="D56" s="44"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="43" t="s">
+      <c r="B56" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="G56" s="44"/>
-      <c r="H56" s="45"/>
-      <c r="J56" s="43" t="s">
+      <c r="C56" s="45"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="K56" s="45"/>
-      <c r="L56" s="43" t="s">
+      <c r="G56" s="45"/>
+      <c r="H56" s="46"/>
+      <c r="J56" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="M56" s="45"/>
+      <c r="K56" s="46"/>
+      <c r="L56" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="M56" s="46"/>
     </row>
     <row r="57" spans="1:14" customHeight="1" ht="12">
-      <c r="B57" s="46"/>
-      <c r="C57" s="47"/>
-      <c r="D57" s="47"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="46"/>
-      <c r="G57" s="47"/>
-      <c r="H57" s="48"/>
-      <c r="J57" s="46"/>
-      <c r="K57" s="48"/>
-      <c r="L57" s="46"/>
-      <c r="M57" s="48"/>
+      <c r="B57" s="47"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="49"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="48"/>
+      <c r="H57" s="49"/>
+      <c r="J57" s="47"/>
+      <c r="K57" s="49"/>
+      <c r="L57" s="47"/>
+      <c r="M57" s="49"/>
     </row>
     <row r="58" spans="1:14" customHeight="1" ht="13.5">
-      <c r="B58" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="C58" s="47"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="48"/>
-      <c r="F58" s="46" t="s">
+      <c r="B58" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="G58" s="47"/>
-      <c r="H58" s="48"/>
-      <c r="J58" s="46" t="s">
+      <c r="C58" s="48"/>
+      <c r="D58" s="48"/>
+      <c r="E58" s="49"/>
+      <c r="F58" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="K58" s="48"/>
-      <c r="L58" s="46" t="s">
+      <c r="G58" s="48"/>
+      <c r="H58" s="49"/>
+      <c r="J58" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="M58" s="48"/>
+      <c r="K58" s="49"/>
+      <c r="L58" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="M58" s="49"/>
     </row>
     <row r="59" spans="1:14" customHeight="1" ht="14.25">
-      <c r="B59" s="46"/>
-      <c r="C59" s="47"/>
-      <c r="D59" s="47"/>
-      <c r="E59" s="48"/>
-      <c r="F59" s="46"/>
-      <c r="G59" s="47"/>
-      <c r="H59" s="48"/>
-      <c r="J59" s="46"/>
-      <c r="K59" s="48"/>
-      <c r="L59" s="46"/>
-      <c r="M59" s="48"/>
+      <c r="B59" s="47"/>
+      <c r="C59" s="48"/>
+      <c r="D59" s="48"/>
+      <c r="E59" s="49"/>
+      <c r="F59" s="47"/>
+      <c r="G59" s="48"/>
+      <c r="H59" s="49"/>
+      <c r="J59" s="47"/>
+      <c r="K59" s="49"/>
+      <c r="L59" s="47"/>
+      <c r="M59" s="49"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="B60" s="59"/>
-      <c r="C60" s="61"/>
-      <c r="D60" s="61"/>
-      <c r="E60" s="60"/>
-      <c r="F60" s="59"/>
-      <c r="G60" s="61"/>
-      <c r="H60" s="61"/>
-      <c r="I60" s="61"/>
-      <c r="J60" s="59"/>
-      <c r="K60" s="60"/>
-      <c r="L60" s="59"/>
-      <c r="M60" s="60"/>
+      <c r="B60" s="60"/>
+      <c r="C60" s="62"/>
+      <c r="D60" s="62"/>
+      <c r="E60" s="61"/>
+      <c r="F60" s="60"/>
+      <c r="G60" s="62"/>
+      <c r="H60" s="62"/>
+      <c r="I60" s="62"/>
+      <c r="J60" s="60"/>
+      <c r="K60" s="61"/>
+      <c r="L60" s="60"/>
+      <c r="M60" s="61"/>
     </row>
     <row r="61" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B61" s="59"/>
-      <c r="C61" s="61"/>
-      <c r="D61" s="61"/>
-      <c r="E61" s="60"/>
-      <c r="F61" s="59"/>
-      <c r="G61" s="61"/>
-      <c r="H61" s="61"/>
-      <c r="I61" s="61"/>
-      <c r="J61" s="59"/>
-      <c r="K61" s="60"/>
-      <c r="L61" s="59"/>
-      <c r="M61" s="60"/>
+      <c r="B61" s="60"/>
+      <c r="C61" s="62"/>
+      <c r="D61" s="62"/>
+      <c r="E61" s="61"/>
+      <c r="F61" s="60"/>
+      <c r="G61" s="62"/>
+      <c r="H61" s="62"/>
+      <c r="I61" s="62"/>
+      <c r="J61" s="60"/>
+      <c r="K61" s="61"/>
+      <c r="L61" s="60"/>
+      <c r="M61" s="61"/>
     </row>
     <row r="62" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B62" s="59"/>
-      <c r="C62" s="61"/>
-      <c r="D62" s="61"/>
-      <c r="E62" s="60"/>
-      <c r="F62" s="59"/>
-      <c r="G62" s="61"/>
-      <c r="H62" s="61"/>
-      <c r="I62" s="61"/>
-      <c r="J62" s="59"/>
-      <c r="K62" s="60"/>
-      <c r="L62" s="59"/>
-      <c r="M62" s="60"/>
+      <c r="B62" s="60"/>
+      <c r="C62" s="62"/>
+      <c r="D62" s="62"/>
+      <c r="E62" s="61"/>
+      <c r="F62" s="60"/>
+      <c r="G62" s="62"/>
+      <c r="H62" s="62"/>
+      <c r="I62" s="62"/>
+      <c r="J62" s="60"/>
+      <c r="K62" s="61"/>
+      <c r="L62" s="60"/>
+      <c r="M62" s="61"/>
     </row>
     <row r="63" spans="1:14" customHeight="1" ht="7.5">
-      <c r="B63" s="59"/>
-      <c r="C63" s="61"/>
-      <c r="D63" s="61"/>
-      <c r="E63" s="60"/>
-      <c r="F63" s="59"/>
-      <c r="G63" s="61"/>
-      <c r="H63" s="61"/>
-      <c r="I63" s="61"/>
-      <c r="J63" s="59"/>
-      <c r="K63" s="60"/>
-      <c r="L63" s="59"/>
-      <c r="M63" s="60"/>
+      <c r="B63" s="60"/>
+      <c r="C63" s="62"/>
+      <c r="D63" s="62"/>
+      <c r="E63" s="61"/>
+      <c r="F63" s="60"/>
+      <c r="G63" s="62"/>
+      <c r="H63" s="62"/>
+      <c r="I63" s="62"/>
+      <c r="J63" s="60"/>
+      <c r="K63" s="61"/>
+      <c r="L63" s="60"/>
+      <c r="M63" s="61"/>
     </row>
     <row r="64" spans="1:14">
       <c r="A64" s="3"/>
-      <c r="B64" s="59"/>
-      <c r="C64" s="61"/>
-      <c r="D64" s="61"/>
-      <c r="E64" s="60"/>
-      <c r="F64" s="59"/>
-      <c r="G64" s="61"/>
-      <c r="H64" s="61"/>
-      <c r="I64" s="61"/>
-      <c r="J64" s="59"/>
-      <c r="K64" s="60"/>
-      <c r="L64" s="59"/>
-      <c r="M64" s="60"/>
+      <c r="B64" s="60"/>
+      <c r="C64" s="62"/>
+      <c r="D64" s="62"/>
+      <c r="E64" s="61"/>
+      <c r="F64" s="60"/>
+      <c r="G64" s="62"/>
+      <c r="H64" s="62"/>
+      <c r="I64" s="62"/>
+      <c r="J64" s="60"/>
+      <c r="K64" s="61"/>
+      <c r="L64" s="60"/>
+      <c r="M64" s="61"/>
     </row>
     <row r="65" spans="1:14" customHeight="1" ht="34.5">
       <c r="A65" s="3"/>
-      <c r="B65" s="59"/>
-      <c r="C65" s="61"/>
-      <c r="D65" s="61"/>
-      <c r="E65" s="60"/>
-      <c r="F65" s="59"/>
-      <c r="G65" s="61"/>
-      <c r="H65" s="61"/>
-      <c r="I65" s="61"/>
-      <c r="J65" s="59"/>
-      <c r="K65" s="60"/>
-      <c r="L65" s="59"/>
-      <c r="M65" s="60"/>
+      <c r="B65" s="60"/>
+      <c r="C65" s="62"/>
+      <c r="D65" s="62"/>
+      <c r="E65" s="61"/>
+      <c r="F65" s="60"/>
+      <c r="G65" s="62"/>
+      <c r="H65" s="62"/>
+      <c r="I65" s="62"/>
+      <c r="J65" s="60"/>
+      <c r="K65" s="61"/>
+      <c r="L65" s="60"/>
+      <c r="M65" s="61"/>
     </row>
     <row r="66" spans="1:14" customHeight="1" ht="12.75">
-      <c r="B66" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="C66" s="63"/>
-      <c r="D66" s="63"/>
-      <c r="E66" s="64"/>
-      <c r="F66" s="57" t="s">
+      <c r="B66" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="G66" s="65"/>
-      <c r="H66" s="58"/>
-      <c r="J66" s="65" t="s">
+      <c r="C66" s="64"/>
+      <c r="D66" s="64"/>
+      <c r="E66" s="65"/>
+      <c r="F66" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="K66" s="58"/>
-      <c r="L66" s="57" t="s">
+      <c r="G66" s="66"/>
+      <c r="H66" s="59"/>
+      <c r="J66" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="M66" s="58"/>
-    </row>
-    <row r="76" spans="1:14">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1" t="s">
+      <c r="K66" s="59"/>
+      <c r="L66" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="L76" s="21"/>
-    </row>
-    <row r="80" spans="1:14" customHeight="1" ht="0.75"/>
-    <row r="81" spans="1:14" hidden="true"/>
+      <c r="M66" s="59"/>
+    </row>
+    <row r="71" spans="1:14">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L71" s="21"/>
+    </row>
+    <row r="75" spans="1:14" customHeight="1" ht="0.75"/>
+    <row r="76" spans="1:14" hidden="true"/>
   </sheetData>
   <mergeCells>
     <mergeCell ref="L66:M66"/>

</xml_diff>

<commit_message>
Wip:se crea formato e insecion para mantenimientos
</commit_message>
<xml_diff>
--- a/imagenes_guardadas/archivo_modificado_RESGUARDO.xlsx
+++ b/imagenes_guardadas/archivo_modificado_RESGUARDO.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>Automóviles y Camiones Rivera, S.A. de C.V.</t>
   </si>
@@ -28,13 +28,13 @@
     <t>No. de Resguardo:</t>
   </si>
   <si>
-    <t>011-00 OTRO</t>
+    <t>01-00 IPAD</t>
   </si>
   <si>
     <t>Fecha de resguardo:</t>
   </si>
   <si>
-    <t>07-FEBRERO-2025</t>
+    <t>10-FEBRERO-2025</t>
   </si>
   <si>
     <t>De acuerdo con la “AS-DV-002. Uso de recursos informáticos”, me comprometo a utilizar el hardware y/o software que se me asigno, exclusivamente para actividades relacionadas con los negocios de la empresa, así como a cuidarlo y mantenerlo en buen estado</t>
@@ -70,16 +70,13 @@
     <t>Inv. Físico</t>
   </si>
   <si>
-    <t>ASDFSA</t>
-  </si>
-  <si>
-    <t>ASDAF</t>
-  </si>
-  <si>
-    <t>ADSF</t>
-  </si>
-  <si>
-    <t>ADFAS</t>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>ENSAMBLE</t>
+  </si>
+  <si>
+    <t>ADSFASFASF</t>
   </si>
   <si>
     <t>N/A</t>
@@ -117,7 +114,7 @@
     <t>Julio Castillo Valerdi</t>
   </si>
   <si>
-    <t>Hj</t>
+    <t>Soporte 1</t>
   </si>
   <si>
     <t>Soporte1</t>
@@ -1348,13 +1345,13 @@
       <c r="I22" s="37"/>
       <c r="J22" s="38"/>
       <c r="K22" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="L22" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="L22" s="25" t="s">
+      <c r="M22" s="19" t="s">
         <v>20</v>
-      </c>
-      <c r="M22" s="19" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:14" customHeight="1" ht="26.25">
@@ -1442,7 +1439,7 @@
     </row>
     <row r="29" spans="1:14" customHeight="1" ht="7.5" hidden="true">
       <c r="B29" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C29" s="29"/>
       <c r="D29" s="29"/>
@@ -1485,7 +1482,7 @@
     <row r="32" spans="1:14" customHeight="1" ht="14.45">
       <c r="A32" s="2"/>
       <c r="B32" s="34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32" s="34"/>
       <c r="D32" s="34"/>
@@ -1502,7 +1499,7 @@
     <row r="33" spans="1:14" customHeight="1" ht="14.45">
       <c r="A33" s="2"/>
       <c r="B33" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="35" t="s">
         <v>12</v>
@@ -1515,10 +1512,10 @@
       <c r="I33" s="35"/>
       <c r="J33" s="35"/>
       <c r="K33" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L33" s="50" t="s">
         <v>25</v>
-      </c>
-      <c r="L33" s="50" t="s">
-        <v>26</v>
       </c>
       <c r="M33" s="51"/>
     </row>
@@ -1578,7 +1575,7 @@
     <row r="41" spans="1:14" customHeight="1" ht="6"/>
     <row r="42" spans="1:14" customHeight="1" ht="13.5">
       <c r="B42" s="42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C42" s="43"/>
       <c r="D42" s="43"/>
@@ -1765,22 +1762,22 @@
     </row>
     <row r="56" spans="1:14" customHeight="1" ht="13.5">
       <c r="B56" s="44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C56" s="45"/>
       <c r="D56" s="45"/>
       <c r="E56" s="46"/>
       <c r="F56" s="44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G56" s="45"/>
       <c r="H56" s="46"/>
       <c r="J56" s="44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K56" s="46"/>
       <c r="L56" s="44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M56" s="46"/>
     </row>
@@ -1799,22 +1796,22 @@
     </row>
     <row r="58" spans="1:14" customHeight="1" ht="13.5">
       <c r="B58" s="47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C58" s="48"/>
       <c r="D58" s="48"/>
       <c r="E58" s="49"/>
       <c r="F58" s="47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G58" s="48"/>
       <c r="H58" s="49"/>
       <c r="J58" s="47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K58" s="49"/>
       <c r="L58" s="47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M58" s="49"/>
     </row>
@@ -1919,29 +1916,29 @@
     </row>
     <row r="66" spans="1:14" customHeight="1" ht="12.75">
       <c r="B66" s="63" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C66" s="64"/>
       <c r="D66" s="64"/>
       <c r="E66" s="65"/>
       <c r="F66" s="58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G66" s="66"/>
       <c r="H66" s="59"/>
       <c r="J66" s="66" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K66" s="59"/>
       <c r="L66" s="58" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M66" s="59"/>
     </row>
     <row r="71" spans="1:14">
       <c r="A71" s="1"/>
       <c r="B71" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L71" s="21"/>
     </row>

</xml_diff>

<commit_message>
se creo final de registro
</commit_message>
<xml_diff>
--- a/imagenes_guardadas/archivo_modificado_RESGUARDO.xlsx
+++ b/imagenes_guardadas/archivo_modificado_RESGUARDO.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>Automóviles y Camiones Rivera, S.A. de C.V.</t>
   </si>
@@ -28,13 +28,13 @@
     <t>No. de Resguardo:</t>
   </si>
   <si>
-    <t>02-00 TABLET</t>
+    <t>023-00 PC-COMPLETA</t>
   </si>
   <si>
     <t>Fecha de resguardo:</t>
   </si>
   <si>
-    <t>11-FEBRERO-2025</t>
+    <t>14-FEBRERO-2025</t>
   </si>
   <si>
     <t>De acuerdo con la “AS-DV-002. Uso de recursos informáticos”, me comprometo a utilizar el hardware y/o software que se me asigno, exclusivamente para actividades relacionadas con los negocios de la empresa, así como a cuidarlo y mantenerlo en buen estado</t>
@@ -70,16 +70,13 @@
     <t>Inv. Físico</t>
   </si>
   <si>
-    <t>ADFA</t>
-  </si>
-  <si>
-    <t>ADSF</t>
-  </si>
-  <si>
-    <t>ADF</t>
-  </si>
-  <si>
-    <t>ASFD</t>
+    <t>ASDSAD</t>
+  </si>
+  <si>
+    <t>ASDASD</t>
+  </si>
+  <si>
+    <t>ASD</t>
   </si>
   <si>
     <t>N/A</t>
@@ -117,7 +114,7 @@
     <t>Julio Castillo Valerdi</t>
   </si>
   <si>
-    <t>Soporte 1</t>
+    <t>Asdad</t>
   </si>
   <si>
     <t>Soporte1</t>
@@ -1333,7 +1330,7 @@
     <row r="22" spans="1:14" customHeight="1" ht="26.25">
       <c r="A22" s="2"/>
       <c r="B22" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" s="39" t="s">
         <v>17</v>
@@ -1351,10 +1348,10 @@
         <v>19</v>
       </c>
       <c r="L22" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="M22" s="19" t="s">
         <v>20</v>
-      </c>
-      <c r="M22" s="19" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:14" customHeight="1" ht="26.25">
@@ -1442,7 +1439,7 @@
     </row>
     <row r="29" spans="1:14" customHeight="1" ht="7.5" hidden="true">
       <c r="B29" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C29" s="29"/>
       <c r="D29" s="29"/>
@@ -1485,7 +1482,7 @@
     <row r="32" spans="1:14" customHeight="1" ht="14.45">
       <c r="A32" s="2"/>
       <c r="B32" s="34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32" s="34"/>
       <c r="D32" s="34"/>
@@ -1502,7 +1499,7 @@
     <row r="33" spans="1:14" customHeight="1" ht="14.45">
       <c r="A33" s="2"/>
       <c r="B33" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="35" t="s">
         <v>12</v>
@@ -1515,10 +1512,10 @@
       <c r="I33" s="35"/>
       <c r="J33" s="35"/>
       <c r="K33" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L33" s="50" t="s">
         <v>25</v>
-      </c>
-      <c r="L33" s="50" t="s">
-        <v>26</v>
       </c>
       <c r="M33" s="51"/>
     </row>
@@ -1578,7 +1575,7 @@
     <row r="41" spans="1:14" customHeight="1" ht="6"/>
     <row r="42" spans="1:14" customHeight="1" ht="13.5">
       <c r="B42" s="42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C42" s="43"/>
       <c r="D42" s="43"/>
@@ -1765,22 +1762,22 @@
     </row>
     <row r="56" spans="1:14" customHeight="1" ht="13.5">
       <c r="B56" s="44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C56" s="45"/>
       <c r="D56" s="45"/>
       <c r="E56" s="46"/>
       <c r="F56" s="44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G56" s="45"/>
       <c r="H56" s="46"/>
       <c r="J56" s="44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K56" s="46"/>
       <c r="L56" s="44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M56" s="46"/>
     </row>
@@ -1799,22 +1796,22 @@
     </row>
     <row r="58" spans="1:14" customHeight="1" ht="13.5">
       <c r="B58" s="47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C58" s="48"/>
       <c r="D58" s="48"/>
       <c r="E58" s="49"/>
       <c r="F58" s="47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G58" s="48"/>
       <c r="H58" s="49"/>
       <c r="J58" s="47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K58" s="49"/>
       <c r="L58" s="47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M58" s="49"/>
     </row>
@@ -1919,29 +1916,29 @@
     </row>
     <row r="66" spans="1:14" customHeight="1" ht="12.75">
       <c r="B66" s="63" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C66" s="64"/>
       <c r="D66" s="64"/>
       <c r="E66" s="65"/>
       <c r="F66" s="58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G66" s="66"/>
       <c r="H66" s="59"/>
       <c r="J66" s="66" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K66" s="59"/>
       <c r="L66" s="58" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M66" s="59"/>
     </row>
     <row r="71" spans="1:14">
       <c r="A71" s="1"/>
       <c r="B71" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L71" s="21"/>
     </row>

</xml_diff>

<commit_message>
se corrige direccion de carpetas en create_registro.php
</commit_message>
<xml_diff>
--- a/imagenes_guardadas/archivo_modificado_RESGUARDO.xlsx
+++ b/imagenes_guardadas/archivo_modificado_RESGUARDO.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>Automóviles y Camiones Rivera, S.A. de C.V.</t>
   </si>
@@ -28,13 +28,13 @@
     <t>No. de Resguardo:</t>
   </si>
   <si>
-    <t>023-00 PC-COMPLETA</t>
+    <t>01-00 MOUSE</t>
   </si>
   <si>
     <t>Fecha de resguardo:</t>
   </si>
   <si>
-    <t>14-FEBRERO-2025</t>
+    <t>01-FEBRERO-2025</t>
   </si>
   <si>
     <t>De acuerdo con la “AS-DV-002. Uso de recursos informáticos”, me comprometo a utilizar el hardware y/o software que se me asigno, exclusivamente para actividades relacionadas con los negocios de la empresa, así como a cuidarlo y mantenerlo en buen estado</t>
@@ -70,13 +70,7 @@
     <t>Inv. Físico</t>
   </si>
   <si>
-    <t>ASDSAD</t>
-  </si>
-  <si>
-    <t>ASDASD</t>
-  </si>
-  <si>
-    <t>ASD</t>
+    <t>GATO</t>
   </si>
   <si>
     <t>N/A</t>
@@ -114,7 +108,7 @@
     <t>Julio Castillo Valerdi</t>
   </si>
   <si>
-    <t>Asdad</t>
+    <t>Sadasd</t>
   </si>
   <si>
     <t>Soporte1</t>
@@ -1339,19 +1333,19 @@
       <c r="E22" s="40"/>
       <c r="F22" s="41"/>
       <c r="G22" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H22" s="37"/>
       <c r="I22" s="37"/>
       <c r="J22" s="38"/>
       <c r="K22" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L22" s="25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M22" s="19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:14" customHeight="1" ht="26.25">
@@ -1439,7 +1433,7 @@
     </row>
     <row r="29" spans="1:14" customHeight="1" ht="7.5" hidden="true">
       <c r="B29" s="29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C29" s="29"/>
       <c r="D29" s="29"/>
@@ -1482,7 +1476,7 @@
     <row r="32" spans="1:14" customHeight="1" ht="14.45">
       <c r="A32" s="2"/>
       <c r="B32" s="34" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C32" s="34"/>
       <c r="D32" s="34"/>
@@ -1499,7 +1493,7 @@
     <row r="33" spans="1:14" customHeight="1" ht="14.45">
       <c r="A33" s="2"/>
       <c r="B33" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C33" s="35" t="s">
         <v>12</v>
@@ -1512,10 +1506,10 @@
       <c r="I33" s="35"/>
       <c r="J33" s="35"/>
       <c r="K33" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L33" s="50" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M33" s="51"/>
     </row>
@@ -1575,7 +1569,7 @@
     <row r="41" spans="1:14" customHeight="1" ht="6"/>
     <row r="42" spans="1:14" customHeight="1" ht="13.5">
       <c r="B42" s="42" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C42" s="43"/>
       <c r="D42" s="43"/>
@@ -1762,22 +1756,22 @@
     </row>
     <row r="56" spans="1:14" customHeight="1" ht="13.5">
       <c r="B56" s="44" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C56" s="45"/>
       <c r="D56" s="45"/>
       <c r="E56" s="46"/>
       <c r="F56" s="44" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G56" s="45"/>
       <c r="H56" s="46"/>
       <c r="J56" s="44" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K56" s="46"/>
       <c r="L56" s="44" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M56" s="46"/>
     </row>
@@ -1796,22 +1790,22 @@
     </row>
     <row r="58" spans="1:14" customHeight="1" ht="13.5">
       <c r="B58" s="47" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C58" s="48"/>
       <c r="D58" s="48"/>
       <c r="E58" s="49"/>
       <c r="F58" s="47" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G58" s="48"/>
       <c r="H58" s="49"/>
       <c r="J58" s="47" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K58" s="49"/>
       <c r="L58" s="47" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M58" s="49"/>
     </row>
@@ -1916,29 +1910,29 @@
     </row>
     <row r="66" spans="1:14" customHeight="1" ht="12.75">
       <c r="B66" s="63" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C66" s="64"/>
       <c r="D66" s="64"/>
       <c r="E66" s="65"/>
       <c r="F66" s="58" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G66" s="66"/>
       <c r="H66" s="59"/>
       <c r="J66" s="66" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K66" s="59"/>
       <c r="L66" s="58" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M66" s="59"/>
     </row>
     <row r="71" spans="1:14">
       <c r="A71" s="1"/>
       <c r="B71" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L71" s="21"/>
     </row>

</xml_diff>